<commit_message>
Update for column names in d18O files.
</commit_message>
<xml_diff>
--- a/Test-Data/WiscSIMSColumnDictionary.xlsx
+++ b/Test-Data/WiscSIMSColumnDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macrostrat/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9F85B6-D528-424D-B726-F6B06BC3788C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D673D1C1-CD0B-3B4C-B8C6-0A03072CCDC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="940" windowWidth="27240" windowHeight="9520" xr2:uid="{D6E065B3-28E8-C041-887D-7F2DC3F0674B}"/>
   </bookViews>
@@ -152,9 +152,6 @@
     <t>DTFAY</t>
   </si>
   <si>
-    <t>\u03B418O \u2030 VSMOW vs UWC-3, d18O \u2030 VSMOW, d18_VSMOW, d18O [VSMOW],d18 VSMOW, \u03B418O \u2030 VSMOW, &lt;U+03B4&gt;18O &lt;U+2030&gt; VSMOW vs UWC-3, δ18O ‰ VSMOW vs UWC-3</t>
-  </si>
-  <si>
     <t>Bias, IMF, Mass Bias (&lt;U+2030&gt;), Mass Bias (‰)</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>2SE (int.), d18O-2SE, d13C-2SE</t>
+  </si>
+  <si>
+    <t>\u03B418O \u2030 VSMOW vs UWC-3, d18O \u2030 VSMOW, d18_VSMOW, d18O [VSMOW],d18 VSMOW, \u03B418O \u2030 VSMOW, &lt;U+03B4&gt;18O &lt;U+2030&gt; VSMOW vs UWC-3, δ18O ‰ VSMOW vs UWC-3, d18O ‰ VSMOW, δ18O ‰ VSMOW</t>
   </si>
 </sst>
 </file>
@@ -684,7 +684,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,10 +705,10 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -722,10 +722,10 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -742,7 +742,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -751,16 +751,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -769,16 +769,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -787,16 +787,16 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -804,16 +804,16 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -821,16 +821,16 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -844,10 +844,10 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -861,28 +861,28 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -897,10 +897,10 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -918,7 +918,7 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -935,7 +935,7 @@
         <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -950,10 +950,10 @@
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -968,10 +968,10 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -986,10 +986,10 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -1004,10 +1004,10 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1021,27 +1021,27 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1055,27 +1055,27 @@
         <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -1084,16 +1084,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1101,13 +1101,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1118,167 +1118,167 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
         <v>2</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D38" t="s">
         <v>34</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" t="s">
         <v>89</v>
       </c>
-      <c r="D39" t="s">
-        <v>90</v>
-      </c>
       <c r="E39" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed mass column requirement
</commit_message>
<xml_diff>
--- a/Test-Data/WiscSIMSColumnDictionary.xlsx
+++ b/Test-Data/WiscSIMSColumnDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macrostrat/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D673D1C1-CD0B-3B4C-B8C6-0A03072CCDC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0573F6DE-58EE-1C4A-B936-B54EAAE292AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="940" windowWidth="27240" windowHeight="9520" xr2:uid="{D6E065B3-28E8-C041-887D-7F2DC3F0674B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="93">
   <si>
     <t>ColNames</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Y, y</t>
   </si>
   <si>
-    <t>Mass</t>
-  </si>
-  <si>
     <t>12CE6</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
   </si>
   <si>
     <t>bits</t>
-  </si>
-  <si>
-    <t>AMU</t>
   </si>
   <si>
     <t>permille_VPDB</t>
@@ -681,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1851B6-D3C4-5D4B-A083-B3E85925BA08}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,10 +699,10 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -722,10 +716,10 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -742,7 +736,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -751,16 +745,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -769,73 +763,73 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -844,15 +838,15 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -861,34 +855,34 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -897,10 +891,10 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -918,12 +912,12 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -932,16 +926,16 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -950,16 +944,16 @@
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -968,132 +962,129 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
-        <v>21</v>
-      </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>92</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1101,184 +1092,170 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
       </c>
       <c r="D24" t="s">
         <v>50</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D37" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" t="s">
         <v>87</v>
       </c>
-      <c r="D38" t="s">
-        <v>34</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>88</v>
-      </c>
-      <c r="D39" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited for d13C file opening
Needs more columns, but a start.
</commit_message>
<xml_diff>
--- a/Test-Data/WiscSIMSColumnDictionary.xlsx
+++ b/Test-Data/WiscSIMSColumnDictionary.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macrostrat/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macrostrat/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0573F6DE-58EE-1C4A-B936-B54EAAE292AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9173F3EB-C8B4-CC49-9863-F270CDBE60A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="940" windowWidth="27240" windowHeight="9520" xr2:uid="{D6E065B3-28E8-C041-887D-7F2DC3F0674B}"/>
   </bookViews>
   <sheets>
     <sheet name="WiscSIMSColumnDictionary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="94">
   <si>
     <t>ColNames</t>
   </si>
@@ -260,12 +260,6 @@
     <t>StdGroup</t>
   </si>
   <si>
-    <t>d13_C</t>
-  </si>
-  <si>
-    <t>d13C_m</t>
-  </si>
-  <si>
     <t>Yield 1MHz/nA</t>
   </si>
   <si>
@@ -312,6 +306,15 @@
   </si>
   <si>
     <t>\u03B418O \u2030 VSMOW vs UWC-3, d18O \u2030 VSMOW, d18_VSMOW, d18O [VSMOW],d18 VSMOW, \u03B418O \u2030 VSMOW, &lt;U+03B4&gt;18O &lt;U+2030&gt; VSMOW vs UWC-3, δ18O ‰ VSMOW vs UWC-3, d18O ‰ VSMOW, δ18O ‰ VSMOW</t>
+  </si>
+  <si>
+    <t>Comment, Comment..2</t>
+  </si>
+  <si>
+    <t>d13C_m, δ13C ‰ measured</t>
+  </si>
+  <si>
+    <t>d13_C, δ13C ‰ VPDB, d13C PDB, δ13C [‰, PDB]</t>
   </si>
 </sst>
 </file>
@@ -677,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1851B6-D3C4-5D4B-A083-B3E85925BA08}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -702,7 +705,7 @@
         <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -716,10 +719,10 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -727,7 +730,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -736,7 +739,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -745,7 +748,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -754,7 +757,7 @@
         <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -763,7 +766,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -772,7 +775,7 @@
         <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -790,7 +793,7 @@
         <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -807,7 +810,7 @@
         <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -815,7 +818,7 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -824,7 +827,7 @@
         <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -841,7 +844,7 @@
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -858,25 +861,25 @@
         <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -894,7 +897,7 @@
         <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -912,7 +915,7 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -929,7 +932,7 @@
         <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -947,7 +950,7 @@
         <v>51</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -965,7 +968,7 @@
         <v>51</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -983,7 +986,7 @@
         <v>52</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -1001,7 +1004,7 @@
         <v>52</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1018,7 +1021,7 @@
         <v>65</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1035,15 +1038,15 @@
         <v>50</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -1052,7 +1055,7 @@
         <v>53</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -1061,7 +1064,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
@@ -1070,7 +1073,7 @@
         <v>53</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1084,7 +1087,7 @@
         <v>49</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1095,13 +1098,13 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
         <v>50</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1112,7 +1115,7 @@
         <v>66</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1123,7 +1126,7 @@
         <v>67</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1134,7 +1137,7 @@
         <v>68</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1145,7 +1148,7 @@
         <v>69</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1156,7 +1159,7 @@
         <v>70</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1167,7 +1170,7 @@
         <v>74</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1178,7 +1181,7 @@
         <v>71</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1189,7 +1192,7 @@
         <v>72</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1200,7 +1203,7 @@
         <v>44</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1211,7 +1214,7 @@
         <v>44</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1222,40 +1225,40 @@
         <v>73</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D36" t="s">
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D37" t="s">
         <v>33</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More changes for d13C data import.
May need more work on d13C importing, but starting to flesh out column dictionary.
</commit_message>
<xml_diff>
--- a/Test-Data/WiscSIMSColumnDictionary.xlsx
+++ b/Test-Data/WiscSIMSColumnDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macrostrat/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9173F3EB-C8B4-CC49-9863-F270CDBE60A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06128AED-D552-5041-A3E9-4D8CBCE65DFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="940" windowWidth="27240" windowHeight="9520" xr2:uid="{D6E065B3-28E8-C041-887D-7F2DC3F0674B}"/>
+    <workbookView xWindow="460" yWindow="940" windowWidth="24360" windowHeight="15480" xr2:uid="{D6E065B3-28E8-C041-887D-7F2DC3F0674B}"/>
   </bookViews>
   <sheets>
     <sheet name="WiscSIMSColumnDictionary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="96">
   <si>
     <t>ColNames</t>
   </si>
@@ -56,45 +56,15 @@
     <t>SIMSmethods</t>
   </si>
   <si>
-    <t>File, Filename</t>
-  </si>
-  <si>
     <t>d18O10</t>
   </si>
   <si>
     <t>Comment</t>
   </si>
   <si>
-    <t>16O (Gcps), 16O(E9 cps), 16O     (E9 cps), 16O (E9), 16O(E9)</t>
-  </si>
-  <si>
-    <t>IP(nA), IP(nA)  1.7 to 1.9, IP (nA)</t>
-  </si>
-  <si>
-    <t>Yield (Gcps/nA), Yield(E9cps/nA), Yield (E9cps/nA)</t>
-  </si>
-  <si>
-    <t>date, Date</t>
-  </si>
-  <si>
-    <t>time, Time</t>
-  </si>
-  <si>
-    <t>X, x</t>
-  </si>
-  <si>
-    <t>d18O10, d13C7</t>
-  </si>
-  <si>
-    <t>Y, y</t>
-  </si>
-  <si>
     <t>12CE6</t>
   </si>
   <si>
-    <t>12C (E6), 12C(E6)</t>
-  </si>
-  <si>
     <t>d13C7</t>
   </si>
   <si>
@@ -110,12 +80,6 @@
     <t>O16(E6)</t>
   </si>
   <si>
-    <t>DTFA-X, DTFA X</t>
-  </si>
-  <si>
-    <t>DTFA-Y, DTFA Y</t>
-  </si>
-  <si>
     <t>IMF</t>
   </si>
   <si>
@@ -149,18 +113,9 @@
     <t>DTFAY</t>
   </si>
   <si>
-    <t>Bias, IMF, Mass Bias (&lt;U+2030&gt;), Mass Bias (‰)</t>
-  </si>
-  <si>
-    <t>d18O ‰ raw, d18O_m, d18O_meas, d18_c, d18O meas, d18O ‰ measured, \u03B418O ‰ measured, &lt;U+03B4&gt;18O &lt;U+2030&gt; measured, δ18O ‰ measured</t>
-  </si>
-  <si>
     <t>Hyd</t>
   </si>
   <si>
-    <t>16OH/16O, 16O1H/16O, 13CH/13C</t>
-  </si>
-  <si>
     <t>13C (cps)</t>
   </si>
   <si>
@@ -266,9 +221,6 @@
     <t>d13CVPDB</t>
   </si>
   <si>
-    <t>2SD (ext.), Er (2S), 2SD, Std_1SD, Er(2S)</t>
-  </si>
-  <si>
     <t>YieldMHz</t>
   </si>
   <si>
@@ -302,19 +254,73 @@
     <t>Numeric</t>
   </si>
   <si>
-    <t>2SE (int.), d18O-2SE, d13C-2SE</t>
-  </si>
-  <si>
-    <t>\u03B418O \u2030 VSMOW vs UWC-3, d18O \u2030 VSMOW, d18_VSMOW, d18O [VSMOW],d18 VSMOW, \u03B418O \u2030 VSMOW, &lt;U+03B4&gt;18O &lt;U+2030&gt; VSMOW vs UWC-3, δ18O ‰ VSMOW vs UWC-3, d18O ‰ VSMOW, δ18O ‰ VSMOW</t>
-  </si>
-  <si>
-    <t>Comment, Comment..2</t>
-  </si>
-  <si>
-    <t>d13C_m, δ13C ‰ measured</t>
-  </si>
-  <si>
-    <t>d13_C, δ13C ‰ VPDB, d13C PDB, δ13C [‰, PDB]</t>
+    <t>File; Filename</t>
+  </si>
+  <si>
+    <t>Comment; Comment..2</t>
+  </si>
+  <si>
+    <t>\u03B418O \u2030 VSMOW vs UWC-3; d18O \u2030 VSMOW; d18_VSMOW; d18O [VSMOW],d18 VSMOW; \u03B418O \u2030 VSMOW; &lt;U+03B4&gt;18O &lt;U+2030&gt; VSMOW vs UWC-3; δ18O ‰ VSMOW vs UWC-3; d18O ‰ VSMOW; δ18O ‰ VSMOW</t>
+  </si>
+  <si>
+    <t>2SD (ext.); Er (2S); 2SD; Std_1SD; Er(2S)</t>
+  </si>
+  <si>
+    <t>Bias; IMF; Mass Bias (&lt;U+2030&gt;); Mass Bias (‰)</t>
+  </si>
+  <si>
+    <t>d18O ‰ raw; d18O_m; d18O_meas; d18_c; d18O meas; d18O ‰ measured; \u03B418O ‰ measured; &lt;U+03B4&gt;18O &lt;U+2030&gt; measured; δ18O ‰ measured</t>
+  </si>
+  <si>
+    <t>2SE (int.); d18O-2SE; d13C-2SE</t>
+  </si>
+  <si>
+    <t>16O (Gcps); 16O(E9 cps); 16O     (E9 cps); 16O (E9); 16O(E9)</t>
+  </si>
+  <si>
+    <t>IP(nA); IP(nA)  1.7 to 1.9; IP (nA)</t>
+  </si>
+  <si>
+    <t>Yield (Gcps/nA); Yield(E9cps/nA); Yield (E9cps/nA)</t>
+  </si>
+  <si>
+    <t>date; Date</t>
+  </si>
+  <si>
+    <t>time; Time</t>
+  </si>
+  <si>
+    <t>X; x</t>
+  </si>
+  <si>
+    <t>Y; y</t>
+  </si>
+  <si>
+    <t>DTFA-X; DTFA X</t>
+  </si>
+  <si>
+    <t>DTFA-Y; DTFA Y</t>
+  </si>
+  <si>
+    <t>16OH/16O; 16O1H/16O; 13CH/13C</t>
+  </si>
+  <si>
+    <t>12C (E6); 12C(E6)</t>
+  </si>
+  <si>
+    <t>d18O10; d13C7</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Mass; mass</t>
+  </si>
+  <si>
+    <t>d13C_m; δ13C ‰ measured; \u03B413C measured; \u03B413C \u2030 measured</t>
+  </si>
+  <si>
+    <t>d13_C; δ13C ‰ VPDB; d13C PDB; δ13C [‰, PDB]; \u03B413C [‰ PDB]; δ13C [‰, VPDB]; \u03B413C [‰, VPDB]; \u03B413C [\u2030, VPDB]; \u03B413C [\u2030, PDB]; ; \u03B413C [\u2030 PDB]</t>
   </si>
 </sst>
 </file>
@@ -678,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1851B6-D3C4-5D4B-A083-B3E85925BA08}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -702,10 +708,10 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -713,33 +719,33 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
         <v>91</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -748,16 +754,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -766,138 +772,138 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -906,359 +912,376 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" t="s">
-        <v>52</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
         <v>50</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>88</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>94</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D38" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding column information for more isotopes.
Fixing column names too for general importer. The is_standard is particularly important.
</commit_message>
<xml_diff>
--- a/Test-Data/WiscSIMSColumnDictionary.xlsx
+++ b/Test-Data/WiscSIMSColumnDictionary.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macrostrat/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06128AED-D552-5041-A3E9-4D8CBCE65DFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{456E1189-71D2-3047-984E-C65F5B691EFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="940" windowWidth="24360" windowHeight="15480" xr2:uid="{D6E065B3-28E8-C041-887D-7F2DC3F0674B}"/>
+    <workbookView xWindow="460" yWindow="940" windowWidth="17620" windowHeight="15480" xr2:uid="{D6E065B3-28E8-C041-887D-7F2DC3F0674B}"/>
   </bookViews>
   <sheets>
     <sheet name="WiscSIMSColumnDictionary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="106">
   <si>
     <t>ColNames</t>
   </si>
@@ -321,6 +321,36 @@
   </si>
   <si>
     <t>d13_C; δ13C ‰ VPDB; d13C PDB; δ13C [‰, PDB]; \u03B413C [‰ PDB]; δ13C [‰, VPDB]; \u03B413C [‰, VPDB]; \u03B413C [\u2030, VPDB]; \u03B413C [\u2030, PDB]; ; \u03B413C [\u2030 PDB]</t>
+  </si>
+  <si>
+    <t>d18O10; d13C7; Ca; CaO</t>
+  </si>
+  <si>
+    <t>d18O10; Ca; CaO</t>
+  </si>
+  <si>
+    <t>d44Cameas</t>
+  </si>
+  <si>
+    <t>Ca; CaO</t>
+  </si>
+  <si>
+    <t>\u03B444Ca \u2030 measured</t>
+  </si>
+  <si>
+    <t>40Ca (Gcps)</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Ca40Cps</t>
+  </si>
+  <si>
+    <t>is_standard</t>
+  </si>
+  <si>
+    <t>Boolean</t>
   </si>
 </sst>
 </file>
@@ -684,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1851B6-D3C4-5D4B-A083-B3E85925BA08}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,7 +752,7 @@
         <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
         <v>65</v>
@@ -739,7 +769,7 @@
         <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -775,7 +805,7 @@
         <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -793,7 +823,7 @@
         <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
@@ -827,7 +857,7 @@
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
@@ -861,7 +891,7 @@
         <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
@@ -897,7 +927,7 @@
         <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -915,7 +945,7 @@
         <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
         <v>2</v>
@@ -932,7 +962,7 @@
         <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -950,7 +980,7 @@
         <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D15" t="s">
         <v>36</v>
@@ -968,7 +998,7 @@
         <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -986,7 +1016,7 @@
         <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
         <v>37</v>
@@ -1004,7 +1034,7 @@
         <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
         <v>37</v>
@@ -1021,7 +1051,7 @@
         <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
         <v>37</v>
@@ -1282,6 +1312,54 @@
       </c>
       <c r="E39" s="2" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>